<commit_message>
Add 2020.05.17 folder of web data mining 1 group.
</commit_message>
<xml_diff>
--- a/读书报告分组提交/web data mining新组1/05.10讨论后的读书报告/2020.05.03读书报告汇总.xlsx
+++ b/读书报告分组提交/web data mining新组1/05.10讨论后的读书报告/2020.05.03读书报告汇总.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\pycharm_home\Reading-Club\读书报告分组提交\web data mining新组1\05.10讨论后的读书报告\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D60A3689-0C20-45EE-96C5-DFA672381425}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FC434C7-5292-4F7B-BAB5-BCDB22AF7543}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
   <si>
     <t>成员</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -151,6 +151,10 @@
   </si>
   <si>
     <t>分章节、分层次、有自己理解</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>有自己理解</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -202,7 +206,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -230,6 +234,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -514,7 +524,7 @@
   <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -534,53 +544,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9" t="s">
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9" t="s">
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="31.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9"/>
-      <c r="B2" s="8" t="s">
+      <c r="A2" s="10"/>
+      <c r="B2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8" t="s">
+      <c r="C2" s="11"/>
+      <c r="D2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8" t="s">
+      <c r="E2" s="11"/>
+      <c r="F2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8" t="s">
+      <c r="G2" s="11"/>
+      <c r="H2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8" t="s">
+      <c r="I2" s="11"/>
+      <c r="J2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="8"/>
-      <c r="L2" s="9"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="10"/>
     </row>
     <row r="3" spans="1:12" ht="28.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
+      <c r="A3" s="10"/>
       <c r="B3" s="2" t="s">
         <v>13</v>
       </c>
@@ -611,7 +621,7 @@
       <c r="K3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="L3" s="9"/>
+      <c r="L3" s="10"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -646,33 +656,68 @@
       </c>
       <c r="J5" s="7"/>
       <c r="K5" s="7"/>
-      <c r="L5" s="4"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L5" s="4">
+        <f>SUM(C5,E5,G5,I5,K5)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="F6" s="5"/>
+      <c r="B6" s="1">
+        <v>0</v>
+      </c>
+      <c r="C6" s="7">
+        <v>25</v>
+      </c>
+      <c r="D6" s="1">
+        <v>3</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="G6" s="7"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="4"/>
+      <c r="H6" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" s="4">
+        <v>4</v>
+      </c>
       <c r="J6" s="7"/>
       <c r="K6" s="7"/>
-      <c r="L6" s="4"/>
+      <c r="L6" s="9">
+        <f t="shared" ref="L6:L9" si="0">SUM(C6,E6,G6,I6,K6)</f>
+        <v>29</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
       <c r="C7" s="7"/>
-      <c r="F7" s="5"/>
+      <c r="D7" s="1">
+        <v>3</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
+      <c r="H7" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="I7" s="7">
+        <v>2</v>
+      </c>
       <c r="J7" s="7"/>
       <c r="K7" s="7"/>
-      <c r="L7" s="4"/>
+      <c r="L7" s="9">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
     </row>
     <row r="8" spans="1:12" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -698,7 +743,10 @@
       </c>
       <c r="J8" s="7"/>
       <c r="K8" s="7"/>
-      <c r="L8" s="4"/>
+      <c r="L8" s="9">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -722,35 +770,43 @@
       <c r="I9" s="4"/>
       <c r="J9" s="7"/>
       <c r="K9" s="7"/>
-      <c r="L9" s="4"/>
+      <c r="L9" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:12" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8" t="s">
+      <c r="C10" s="11"/>
+      <c r="D10" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8" t="s">
+      <c r="E10" s="11"/>
+      <c r="F10" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8" t="s">
+      <c r="G10" s="11"/>
+      <c r="H10" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8" t="s">
+      <c r="I10" s="11"/>
+      <c r="J10" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="K10" s="8"/>
+      <c r="K10" s="11"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:L9">
     <sortCondition descending="1" ref="L4:L9"/>
   </sortState>
   <mergeCells count="14">
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="J10:K10"/>
     <mergeCell ref="L1:L3"/>
     <mergeCell ref="B1:G1"/>
     <mergeCell ref="A1:A3"/>
@@ -760,11 +816,6 @@
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="H1:K1"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="J10:K10"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add 2020.05.24 folder of web data mining 1 group.
</commit_message>
<xml_diff>
--- a/读书报告分组提交/web data mining新组1/05.10讨论后的读书报告/2020.05.03读书报告汇总.xlsx
+++ b/读书报告分组提交/web data mining新组1/05.10讨论后的读书报告/2020.05.03读书报告汇总.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\pycharm_home\Reading-Club\读书报告分组提交\web data mining新组1\05.10讨论后的读书报告\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA5AD9AD-379A-47DD-B733-2781F11853E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{952BA339-6F3F-4901-B107-17075820BE44}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="3048" yWindow="3540" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="33">
   <si>
     <t>成员</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -151,6 +151,10 @@
   </si>
   <si>
     <t>有自己理解</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>无</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -202,7 +206,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -226,16 +230,19 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -520,7 +527,7 @@
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -540,29 +547,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10" t="s">
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10" t="s">
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="31.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
+      <c r="A2" s="12"/>
       <c r="B2" s="11" t="s">
         <v>1</v>
       </c>
@@ -583,10 +590,10 @@
         <v>5</v>
       </c>
       <c r="K2" s="11"/>
-      <c r="L2" s="10"/>
+      <c r="L2" s="12"/>
     </row>
     <row r="3" spans="1:12" ht="28.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
+      <c r="A3" s="12"/>
       <c r="B3" s="2" t="s">
         <v>12</v>
       </c>
@@ -617,7 +624,7 @@
       <c r="K3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="10"/>
+      <c r="L3" s="12"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -647,24 +654,26 @@
       <c r="I4" s="7">
         <v>3</v>
       </c>
-      <c r="J4" s="7">
+      <c r="J4" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" s="7">
         <v>0</v>
       </c>
-      <c r="K4" s="7"/>
       <c r="L4" s="4">
         <f>SUM(C4,E4,G4,I4,K4)</f>
         <v>93</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" s="7">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="D5" s="1">
         <v>3</v>
@@ -675,27 +684,29 @@
       <c r="F5" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="8">
         <v>15</v>
       </c>
-      <c r="H5" s="8" t="s">
-        <v>30</v>
+      <c r="H5" s="9" t="s">
+        <v>31</v>
       </c>
       <c r="I5" s="4">
-        <v>4</v>
-      </c>
-      <c r="J5" s="7">
+        <v>2</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="K5" s="9">
         <v>0</v>
       </c>
-      <c r="K5" s="7"/>
-      <c r="L5" s="9">
-        <f t="shared" ref="L5:L8" si="0">SUM(C5,E5,G5,I5,K5)</f>
-        <v>79</v>
+      <c r="L5" s="8">
+        <f>SUM(C5,E5,G5,I5,K5)</f>
+        <v>92</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
@@ -704,33 +715,37 @@
         <v>40</v>
       </c>
       <c r="D6" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E6" s="1">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G6" s="8">
         <v>15</v>
       </c>
-      <c r="H6" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="I6" s="7">
-        <v>2</v>
-      </c>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="9">
-        <f t="shared" si="0"/>
-        <v>92</v>
+      <c r="H6" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" s="10">
+        <v>4</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="K6" s="9">
+        <v>0</v>
+      </c>
+      <c r="L6" s="8">
+        <f>SUM(C6,E6,G6,I6,K6)</f>
+        <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
@@ -747,55 +762,63 @@
       <c r="F7" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="G7" s="9">
+      <c r="G7" s="8">
         <v>15</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="I7" s="6">
-        <v>4</v>
-      </c>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="9">
-        <f t="shared" si="0"/>
-        <v>89</v>
+        <v>28</v>
+      </c>
+      <c r="I7" s="9">
+        <v>0</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="K7" s="9">
+        <v>0</v>
+      </c>
+      <c r="L7" s="8">
+        <f>SUM(C7,E7,G7,I7,K7)</f>
+        <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B8" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" s="7">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="D8" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E8" s="3">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="8">
         <v>15</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="I8" s="4">
+        <v>4</v>
+      </c>
+      <c r="J8" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="K8" s="9">
         <v>0</v>
       </c>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="9">
-        <f t="shared" si="0"/>
-        <v>85</v>
+      <c r="L8" s="8">
+        <f>SUM(C8,E8,G8,I8,K8)</f>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -822,14 +845,9 @@
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:L8">
-    <sortCondition descending="1" ref="L4:L8"/>
+    <sortCondition descending="1" ref="L8"/>
   </sortState>
   <mergeCells count="14">
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="J9:K9"/>
     <mergeCell ref="L1:L3"/>
     <mergeCell ref="B1:G1"/>
     <mergeCell ref="A1:A3"/>
@@ -839,6 +857,11 @@
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="H1:K1"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="J9:K9"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>